<commit_message>
added constraint on nb of months of pregnancy
</commit_message>
<xml_diff>
--- a/xforms/xlsforms/pregnancy_observation.xlsx
+++ b/xforms/xlsforms/pregnancy_observation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
   <si>
     <t>type</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>concat(${individualId},'_OBS_',${fieldWorkerId})</t>
+  </si>
+  <si>
+    <t>.&lt;10</t>
   </si>
 </sst>
 </file>
@@ -1493,11 +1496,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="101" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1766,7 +1769,9 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="b">
         <v>1</v>

</xml_diff>